<commit_message>
test #8: ERROR dado zipfile.BadZipFile: File is not a zip file
</commit_message>
<xml_diff>
--- a/decide/excel/testImport.xlsx
+++ b/decide/excel/testImport.xlsx
@@ -22,37 +22,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
+    <t xml:space="preserve">voting_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
     <t xml:space="preserve">voter_id</t>
   </si>
   <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">voting_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marina</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">Juanjo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rubén</t>
   </si>
   <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juanjo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laura</t>
   </si>
 </sst>
 </file>
@@ -156,10 +156,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -177,7 +177,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -200,26 +200,26 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -228,21 +228,21 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>